<commit_message>
escalation added,report two grapg for total count and difect count
</commit_message>
<xml_diff>
--- a/templates/Excel/AHP_Revision_Histroy.xlsx
+++ b/templates/Excel/AHP_Revision_Histroy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suriya.Prakash\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9419C39-EE8C-4D87-B501-18012B569062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59A5B7E-D2E3-4608-97BA-0BE1D132A5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">Laser Marking Check Point added &amp; Vibrow Machine Check point added </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>3rd station Leakage test stabilization, Test time changed &amp; Spring seat run out check point added</t>
   </si>
@@ -79,6 +76,36 @@
   </si>
   <si>
     <t>Revision Date</t>
+  </si>
+  <si>
+    <t>Station Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laser Marking Check Point added &amp; Vibrotary Machine Check point added </t>
+  </si>
+  <si>
+    <t>Laser Marking &amp; Lipring &amp; Spring seat assembly</t>
+  </si>
+  <si>
+    <t>Cap Handle &amp; Threaded Ferrule sub assembly</t>
+  </si>
+  <si>
+    <t>Rotary table</t>
+  </si>
+  <si>
+    <t>Lipring &amp; Spring seat assembly</t>
+  </si>
+  <si>
+    <t>Process Number</t>
+  </si>
+  <si>
+    <t>80 &amp; 50</t>
+  </si>
+  <si>
+    <t>20.07.2022</t>
+  </si>
+  <si>
+    <t>02.11.2022</t>
   </si>
 </sst>
 </file>
@@ -101,7 +128,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -122,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -220,41 +247,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,127 +598,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="79" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="79" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>60</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9">
-        <v>44762</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="E3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>60</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>44867</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>60</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="B6" s="8">
+        <v>60</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>70</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <v>60</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>60</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>